<commit_message>
Entered through the Baritone Section.
</commit_message>
<xml_diff>
--- a/attendance_issue.xlsx
+++ b/attendance_issue.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csyers\Documents\Fall 2016\Database Concepts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\ND '16-'17\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>NetID</t>
   </si>
@@ -36,6 +36,60 @@
   </si>
   <si>
     <t>Excused</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>mcapella</t>
+  </si>
+  <si>
+    <t>Jessup, Harrison</t>
+  </si>
+  <si>
+    <t>cmulholl</t>
+  </si>
+  <si>
+    <t>joneil11</t>
+  </si>
+  <si>
+    <t>jrudlof2</t>
+  </si>
+  <si>
+    <t>Glaser, Andrew</t>
+  </si>
+  <si>
+    <t>jvander4</t>
+  </si>
+  <si>
+    <t>dconnel5</t>
+  </si>
+  <si>
+    <t>eglaser</t>
+  </si>
+  <si>
+    <t>jlombar2</t>
+  </si>
+  <si>
+    <t>McKenna, Kiera</t>
+  </si>
+  <si>
+    <t>jthesing</t>
+  </si>
+  <si>
+    <t>mwang7</t>
   </si>
 </sst>
 </file>
@@ -387,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -412,6 +466,482 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed the spelling of Dominic Iannelli's netID.
</commit_message>
<xml_diff>
--- a/attendance_issue.xlsx
+++ b/attendance_issue.xlsx
@@ -611,9 +611,6 @@
     <t>cgeary1</t>
   </si>
   <si>
-    <t>dianell</t>
-  </si>
-  <si>
     <t>lunruh1</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>sfrick</t>
+  </si>
+  <si>
+    <t>riannell</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D871"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A589" workbookViewId="0">
+      <selection activeCell="E597" sqref="E597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8989,7 +8989,7 @@
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="B556">
         <v>17</v>
@@ -9017,7 +9017,7 @@
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B558">
         <v>17</v>
@@ -9045,7 +9045,7 @@
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B560">
         <v>20</v>
@@ -9087,7 +9087,7 @@
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B563">
         <v>22</v>
@@ -9101,7 +9101,7 @@
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B564">
         <v>23</v>
@@ -9129,7 +9129,7 @@
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B566">
         <v>23</v>
@@ -9143,7 +9143,7 @@
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B567">
         <v>23</v>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B570">
         <v>24</v>
@@ -9199,7 +9199,7 @@
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B571">
         <v>24</v>
@@ -9213,7 +9213,7 @@
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="B572">
         <v>25</v>
@@ -9241,7 +9241,7 @@
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B574">
         <v>25</v>
@@ -9269,7 +9269,7 @@
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B576">
         <v>27</v>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B579">
         <v>29</v>
@@ -9325,7 +9325,7 @@
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B580">
         <v>29</v>
@@ -9339,7 +9339,7 @@
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B581">
         <v>30</v>
@@ -9395,7 +9395,7 @@
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B585">
         <v>30</v>
@@ -9409,7 +9409,7 @@
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="B586">
         <v>31</v>
@@ -9423,7 +9423,7 @@
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B587">
         <v>31</v>
@@ -9493,7 +9493,7 @@
     </row>
     <row r="592" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B592">
         <v>33</v>
@@ -9535,7 +9535,7 @@
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B595">
         <v>34</v>
@@ -9549,7 +9549,7 @@
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B596">
         <v>36</v>
@@ -9577,7 +9577,7 @@
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B598">
         <v>36</v>
@@ -9605,7 +9605,7 @@
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B600">
         <v>38</v>
@@ -9619,7 +9619,7 @@
     </row>
     <row r="601" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>195</v>
+        <v>276</v>
       </c>
       <c r="B601">
         <v>38</v>
@@ -9633,7 +9633,7 @@
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B602">
         <v>38</v>
@@ -9647,7 +9647,7 @@
     </row>
     <row r="603" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B603">
         <v>38</v>
@@ -9661,7 +9661,7 @@
     </row>
     <row r="604" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B604">
         <v>39</v>
@@ -9675,7 +9675,7 @@
     </row>
     <row r="605" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B605">
         <v>39</v>
@@ -9787,7 +9787,7 @@
     </row>
     <row r="613" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B613">
         <v>45</v>
@@ -9801,7 +9801,7 @@
     </row>
     <row r="614" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B614">
         <v>45</v>
@@ -9815,7 +9815,7 @@
     </row>
     <row r="615" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B615">
         <v>46</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B617">
         <v>46</v>
@@ -9857,7 +9857,7 @@
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B618">
         <v>46</v>
@@ -9885,7 +9885,7 @@
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B620">
         <v>46</v>
@@ -9913,7 +9913,7 @@
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B622">
         <v>46</v>
@@ -9941,7 +9941,7 @@
     </row>
     <row r="624" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B624">
         <v>50</v>
@@ -9955,7 +9955,7 @@
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B625">
         <v>50</v>
@@ -9969,7 +9969,7 @@
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B626">
         <v>50</v>
@@ -9983,7 +9983,7 @@
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B627">
         <v>51</v>
@@ -9997,7 +9997,7 @@
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B628">
         <v>51</v>
@@ -10025,7 +10025,7 @@
     </row>
     <row r="630" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B630">
         <v>51</v>
@@ -10039,7 +10039,7 @@
     </row>
     <row r="631" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B631">
         <v>51</v>
@@ -10053,7 +10053,7 @@
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B632">
         <v>51</v>
@@ -10109,7 +10109,7 @@
     </row>
     <row r="636" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B636">
         <v>51</v>
@@ -10123,7 +10123,7 @@
     </row>
     <row r="637" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B637">
         <v>52</v>
@@ -10151,7 +10151,7 @@
     </row>
     <row r="639" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B639">
         <v>53</v>
@@ -10165,7 +10165,7 @@
     </row>
     <row r="640" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B640">
         <v>55</v>
@@ -10179,7 +10179,7 @@
     </row>
     <row r="641" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B641">
         <v>64</v>
@@ -10207,7 +10207,7 @@
     </row>
     <row r="643" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B643">
         <v>64</v>
@@ -10221,7 +10221,7 @@
     </row>
     <row r="644" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B644">
         <v>64</v>
@@ -10235,7 +10235,7 @@
     </row>
     <row r="645" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B645">
         <v>1</v>
@@ -10249,7 +10249,7 @@
     </row>
     <row r="646" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B646">
         <v>2</v>
@@ -10263,7 +10263,7 @@
     </row>
     <row r="647" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B647">
         <v>2</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="648" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B648">
         <v>2</v>
@@ -10291,7 +10291,7 @@
     </row>
     <row r="649" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B649">
         <v>2</v>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="650" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B650">
         <v>2</v>
@@ -10319,7 +10319,7 @@
     </row>
     <row r="651" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B651">
         <v>2</v>
@@ -10333,7 +10333,7 @@
     </row>
     <row r="652" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B652">
         <v>3</v>
@@ -10347,7 +10347,7 @@
     </row>
     <row r="653" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B653">
         <v>3</v>
@@ -10361,7 +10361,7 @@
     </row>
     <row r="654" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B654">
         <v>3</v>
@@ -10375,7 +10375,7 @@
     </row>
     <row r="655" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B655">
         <v>3</v>
@@ -10389,7 +10389,7 @@
     </row>
     <row r="656" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B656">
         <v>3</v>
@@ -10403,7 +10403,7 @@
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B657">
         <v>3</v>
@@ -10417,7 +10417,7 @@
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B658">
         <v>4</v>
@@ -10431,7 +10431,7 @@
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B659">
         <v>4</v>
@@ -10445,7 +10445,7 @@
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B660">
         <v>4</v>
@@ -10459,7 +10459,7 @@
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B661">
         <v>4</v>
@@ -10473,7 +10473,7 @@
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B662">
         <v>5</v>
@@ -10487,7 +10487,7 @@
     </row>
     <row r="663" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B663">
         <v>5</v>
@@ -10501,7 +10501,7 @@
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B664">
         <v>5</v>
@@ -10515,7 +10515,7 @@
     </row>
     <row r="665" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B665">
         <v>5</v>
@@ -10529,7 +10529,7 @@
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B666">
         <v>5</v>
@@ -10543,7 +10543,7 @@
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B667">
         <v>5</v>
@@ -10557,7 +10557,7 @@
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B668">
         <v>5</v>
@@ -10571,7 +10571,7 @@
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B669">
         <v>5</v>
@@ -10585,7 +10585,7 @@
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B670">
         <v>8</v>
@@ -10599,7 +10599,7 @@
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B671">
         <v>8</v>
@@ -10613,7 +10613,7 @@
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B672">
         <v>8</v>
@@ -10627,7 +10627,7 @@
     </row>
     <row r="673" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B673">
         <v>8</v>
@@ -10641,7 +10641,7 @@
     </row>
     <row r="674" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B674">
         <v>8</v>
@@ -10655,7 +10655,7 @@
     </row>
     <row r="675" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B675">
         <v>9</v>
@@ -10669,7 +10669,7 @@
     </row>
     <row r="676" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B676">
         <v>9</v>
@@ -10683,7 +10683,7 @@
     </row>
     <row r="677" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B677">
         <v>10</v>
@@ -10697,7 +10697,7 @@
     </row>
     <row r="678" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B678">
         <v>10</v>
@@ -10711,7 +10711,7 @@
     </row>
     <row r="679" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B679">
         <v>10</v>
@@ -10725,7 +10725,7 @@
     </row>
     <row r="680" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B680">
         <v>10</v>
@@ -10739,7 +10739,7 @@
     </row>
     <row r="681" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B681">
         <v>10</v>
@@ -10753,7 +10753,7 @@
     </row>
     <row r="682" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B682">
         <v>10</v>
@@ -10767,7 +10767,7 @@
     </row>
     <row r="683" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B683">
         <v>10</v>
@@ -10781,7 +10781,7 @@
     </row>
     <row r="684" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B684">
         <v>11</v>
@@ -10795,7 +10795,7 @@
     </row>
     <row r="685" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B685">
         <v>11</v>
@@ -10809,7 +10809,7 @@
     </row>
     <row r="686" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B686">
         <v>11</v>
@@ -10823,7 +10823,7 @@
     </row>
     <row r="687" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B687">
         <v>11</v>
@@ -10837,7 +10837,7 @@
     </row>
     <row r="688" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B688">
         <v>11</v>
@@ -10851,7 +10851,7 @@
     </row>
     <row r="689" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B689">
         <v>11</v>
@@ -10865,7 +10865,7 @@
     </row>
     <row r="690" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B690">
         <v>11</v>
@@ -10879,7 +10879,7 @@
     </row>
     <row r="691" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B691">
         <v>15</v>
@@ -10893,7 +10893,7 @@
     </row>
     <row r="692" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B692">
         <v>15</v>
@@ -10907,7 +10907,7 @@
     </row>
     <row r="693" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B693">
         <v>15</v>
@@ -10921,7 +10921,7 @@
     </row>
     <row r="694" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B694">
         <v>15</v>
@@ -10935,7 +10935,7 @@
     </row>
     <row r="695" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B695">
         <v>15</v>
@@ -10949,7 +10949,7 @@
     </row>
     <row r="696" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B696">
         <v>15</v>
@@ -10963,7 +10963,7 @@
     </row>
     <row r="697" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B697">
         <v>15</v>
@@ -10977,7 +10977,7 @@
     </row>
     <row r="698" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B698">
         <v>15</v>
@@ -10991,7 +10991,7 @@
     </row>
     <row r="699" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B699">
         <v>16</v>
@@ -11005,7 +11005,7 @@
     </row>
     <row r="700" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B700">
         <v>16</v>
@@ -11019,7 +11019,7 @@
     </row>
     <row r="701" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B701">
         <v>16</v>
@@ -11033,7 +11033,7 @@
     </row>
     <row r="702" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B702">
         <v>16</v>
@@ -11047,7 +11047,7 @@
     </row>
     <row r="703" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B703">
         <v>16</v>
@@ -11061,7 +11061,7 @@
     </row>
     <row r="704" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B704">
         <v>16</v>
@@ -11075,7 +11075,7 @@
     </row>
     <row r="705" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B705">
         <v>17</v>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="706" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B706">
         <v>17</v>
@@ -11103,7 +11103,7 @@
     </row>
     <row r="707" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B707">
         <v>17</v>
@@ -11117,7 +11117,7 @@
     </row>
     <row r="708" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B708">
         <v>17</v>
@@ -11131,7 +11131,7 @@
     </row>
     <row r="709" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B709">
         <v>17</v>
@@ -11145,7 +11145,7 @@
     </row>
     <row r="710" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B710">
         <v>17</v>
@@ -11159,7 +11159,7 @@
     </row>
     <row r="711" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B711">
         <v>18</v>
@@ -11173,7 +11173,7 @@
     </row>
     <row r="712" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B712">
         <v>18</v>
@@ -11187,7 +11187,7 @@
     </row>
     <row r="713" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B713">
         <v>22</v>
@@ -11201,7 +11201,7 @@
     </row>
     <row r="714" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B714">
         <v>22</v>
@@ -11215,7 +11215,7 @@
     </row>
     <row r="715" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B715">
         <v>22</v>
@@ -11229,7 +11229,7 @@
     </row>
     <row r="716" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B716">
         <v>22</v>
@@ -11243,7 +11243,7 @@
     </row>
     <row r="717" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B717">
         <v>22</v>
@@ -11257,7 +11257,7 @@
     </row>
     <row r="718" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B718">
         <v>22</v>
@@ -11271,7 +11271,7 @@
     </row>
     <row r="719" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B719">
         <v>22</v>
@@ -11285,7 +11285,7 @@
     </row>
     <row r="720" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B720">
         <v>22</v>
@@ -11299,7 +11299,7 @@
     </row>
     <row r="721" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B721">
         <v>22</v>
@@ -11313,7 +11313,7 @@
     </row>
     <row r="722" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B722">
         <v>23</v>
@@ -11327,7 +11327,7 @@
     </row>
     <row r="723" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B723">
         <v>23</v>
@@ -11341,7 +11341,7 @@
     </row>
     <row r="724" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B724">
         <v>23</v>
@@ -11355,7 +11355,7 @@
     </row>
     <row r="725" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B725">
         <v>23</v>
@@ -11369,7 +11369,7 @@
     </row>
     <row r="726" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B726">
         <v>23</v>
@@ -11383,7 +11383,7 @@
     </row>
     <row r="727" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B727">
         <v>24</v>
@@ -11397,7 +11397,7 @@
     </row>
     <row r="728" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B728">
         <v>24</v>
@@ -11411,7 +11411,7 @@
     </row>
     <row r="729" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B729">
         <v>24</v>
@@ -11425,7 +11425,7 @@
     </row>
     <row r="730" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B730">
         <v>24</v>
@@ -11439,7 +11439,7 @@
     </row>
     <row r="731" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B731">
         <v>24</v>
@@ -11453,7 +11453,7 @@
     </row>
     <row r="732" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B732">
         <v>24</v>
@@ -11467,7 +11467,7 @@
     </row>
     <row r="733" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B733">
         <v>24</v>
@@ -11481,7 +11481,7 @@
     </row>
     <row r="734" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B734">
         <v>25</v>
@@ -11495,7 +11495,7 @@
     </row>
     <row r="735" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B735">
         <v>25</v>
@@ -11509,7 +11509,7 @@
     </row>
     <row r="736" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B736">
         <v>25</v>
@@ -11523,7 +11523,7 @@
     </row>
     <row r="737" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B737">
         <v>25</v>
@@ -11537,7 +11537,7 @@
     </row>
     <row r="738" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B738">
         <v>25</v>
@@ -11551,7 +11551,7 @@
     </row>
     <row r="739" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B739">
         <v>25</v>
@@ -11565,7 +11565,7 @@
     </row>
     <row r="740" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B740">
         <v>25</v>
@@ -11579,7 +11579,7 @@
     </row>
     <row r="741" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B741">
         <v>25</v>
@@ -11593,7 +11593,7 @@
     </row>
     <row r="742" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B742">
         <v>27</v>
@@ -11607,7 +11607,7 @@
     </row>
     <row r="743" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B743">
         <v>27</v>
@@ -11621,7 +11621,7 @@
     </row>
     <row r="744" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B744">
         <v>29</v>
@@ -11635,7 +11635,7 @@
     </row>
     <row r="745" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B745">
         <v>29</v>
@@ -11649,7 +11649,7 @@
     </row>
     <row r="746" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B746">
         <v>29</v>
@@ -11663,7 +11663,7 @@
     </row>
     <row r="747" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B747">
         <v>29</v>
@@ -11677,7 +11677,7 @@
     </row>
     <row r="748" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B748">
         <v>29</v>
@@ -11691,7 +11691,7 @@
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B749">
         <v>29</v>
@@ -11705,7 +11705,7 @@
     </row>
     <row r="750" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B750">
         <v>30</v>
@@ -11719,7 +11719,7 @@
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B751">
         <v>30</v>
@@ -11733,7 +11733,7 @@
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B752">
         <v>30</v>
@@ -11747,7 +11747,7 @@
     </row>
     <row r="753" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B753">
         <v>30</v>
@@ -11761,7 +11761,7 @@
     </row>
     <row r="754" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B754">
         <v>30</v>
@@ -11775,7 +11775,7 @@
     </row>
     <row r="755" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B755">
         <v>30</v>
@@ -11789,7 +11789,7 @@
     </row>
     <row r="756" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B756">
         <v>30</v>
@@ -11803,7 +11803,7 @@
     </row>
     <row r="757" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B757">
         <v>31</v>
@@ -11817,7 +11817,7 @@
     </row>
     <row r="758" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B758">
         <v>31</v>
@@ -11831,7 +11831,7 @@
     </row>
     <row r="759" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B759">
         <v>31</v>
@@ -11845,7 +11845,7 @@
     </row>
     <row r="760" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B760">
         <v>31</v>
@@ -11859,7 +11859,7 @@
     </row>
     <row r="761" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B761">
         <v>31</v>
@@ -11873,7 +11873,7 @@
     </row>
     <row r="762" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B762">
         <v>31</v>
@@ -11887,7 +11887,7 @@
     </row>
     <row r="763" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B763">
         <v>32</v>
@@ -11901,7 +11901,7 @@
     </row>
     <row r="764" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B764">
         <v>32</v>
@@ -11915,7 +11915,7 @@
     </row>
     <row r="765" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B765">
         <v>32</v>
@@ -11929,7 +11929,7 @@
     </row>
     <row r="766" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B766">
         <v>32</v>
@@ -11943,7 +11943,7 @@
     </row>
     <row r="767" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B767">
         <v>32</v>
@@ -11957,7 +11957,7 @@
     </row>
     <row r="768" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B768">
         <v>32</v>
@@ -11971,7 +11971,7 @@
     </row>
     <row r="769" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B769">
         <v>36</v>
@@ -11985,7 +11985,7 @@
     </row>
     <row r="770" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B770">
         <v>36</v>
@@ -11999,7 +11999,7 @@
     </row>
     <row r="771" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B771">
         <v>36</v>
@@ -12013,7 +12013,7 @@
     </row>
     <row r="772" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B772">
         <v>36</v>
@@ -12027,7 +12027,7 @@
     </row>
     <row r="773" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B773">
         <v>37</v>
@@ -12041,7 +12041,7 @@
     </row>
     <row r="774" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B774">
         <v>37</v>
@@ -12055,7 +12055,7 @@
     </row>
     <row r="775" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B775">
         <v>37</v>
@@ -12069,7 +12069,7 @@
     </row>
     <row r="776" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B776">
         <v>37</v>
@@ -12083,7 +12083,7 @@
     </row>
     <row r="777" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B777">
         <v>37</v>
@@ -12097,7 +12097,7 @@
     </row>
     <row r="778" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B778">
         <v>37</v>
@@ -12111,7 +12111,7 @@
     </row>
     <row r="779" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B779">
         <v>38</v>
@@ -12125,7 +12125,7 @@
     </row>
     <row r="780" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B780">
         <v>38</v>
@@ -12139,7 +12139,7 @@
     </row>
     <row r="781" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B781">
         <v>38</v>
@@ -12153,7 +12153,7 @@
     </row>
     <row r="782" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B782">
         <v>38</v>
@@ -12167,7 +12167,7 @@
     </row>
     <row r="783" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B783">
         <v>38</v>
@@ -12181,7 +12181,7 @@
     </row>
     <row r="784" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B784">
         <v>38</v>
@@ -12195,7 +12195,7 @@
     </row>
     <row r="785" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B785">
         <v>38</v>
@@ -12209,7 +12209,7 @@
     </row>
     <row r="786" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B786">
         <v>38</v>
@@ -12223,7 +12223,7 @@
     </row>
     <row r="787" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B787">
         <v>38</v>
@@ -12237,7 +12237,7 @@
     </row>
     <row r="788" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B788">
         <v>38</v>
@@ -12251,7 +12251,7 @@
     </row>
     <row r="789" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B789">
         <v>38</v>
@@ -12265,7 +12265,7 @@
     </row>
     <row r="790" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B790">
         <v>38</v>
@@ -12279,7 +12279,7 @@
     </row>
     <row r="791" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B791">
         <v>38</v>
@@ -12293,7 +12293,7 @@
     </row>
     <row r="792" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B792">
         <v>38</v>
@@ -12307,7 +12307,7 @@
     </row>
     <row r="793" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B793">
         <v>39</v>
@@ -12321,7 +12321,7 @@
     </row>
     <row r="794" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B794">
         <v>39</v>
@@ -12335,7 +12335,7 @@
     </row>
     <row r="795" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B795">
         <v>39</v>
@@ -12349,7 +12349,7 @@
     </row>
     <row r="796" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B796">
         <v>39</v>
@@ -12363,7 +12363,7 @@
     </row>
     <row r="797" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B797">
         <v>39</v>
@@ -12377,7 +12377,7 @@
     </row>
     <row r="798" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B798">
         <v>39</v>
@@ -12391,7 +12391,7 @@
     </row>
     <row r="799" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B799">
         <v>39</v>
@@ -12405,7 +12405,7 @@
     </row>
     <row r="800" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B800">
         <v>39</v>
@@ -12419,7 +12419,7 @@
     </row>
     <row r="801" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B801">
         <v>39</v>
@@ -12433,7 +12433,7 @@
     </row>
     <row r="802" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B802">
         <v>39</v>
@@ -12447,7 +12447,7 @@
     </row>
     <row r="803" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B803">
         <v>43</v>
@@ -12461,7 +12461,7 @@
     </row>
     <row r="804" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B804">
         <v>43</v>
@@ -12475,7 +12475,7 @@
     </row>
     <row r="805" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B805">
         <v>43</v>
@@ -12489,7 +12489,7 @@
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B806">
         <v>43</v>
@@ -12503,7 +12503,7 @@
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B807">
         <v>44</v>
@@ -12517,7 +12517,7 @@
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B808">
         <v>44</v>
@@ -12531,7 +12531,7 @@
     </row>
     <row r="809" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B809">
         <v>44</v>
@@ -12545,7 +12545,7 @@
     </row>
     <row r="810" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B810">
         <v>45</v>
@@ -12559,7 +12559,7 @@
     </row>
     <row r="811" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B811">
         <v>45</v>
@@ -12573,7 +12573,7 @@
     </row>
     <row r="812" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B812">
         <v>45</v>
@@ -12587,7 +12587,7 @@
     </row>
     <row r="813" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B813">
         <v>45</v>
@@ -12601,7 +12601,7 @@
     </row>
     <row r="814" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B814">
         <v>45</v>
@@ -12615,7 +12615,7 @@
     </row>
     <row r="815" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B815">
         <v>45</v>
@@ -12629,7 +12629,7 @@
     </row>
     <row r="816" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B816">
         <v>46</v>
@@ -12643,7 +12643,7 @@
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B817">
         <v>46</v>
@@ -12657,7 +12657,7 @@
     </row>
     <row r="818" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B818">
         <v>46</v>
@@ -12671,7 +12671,7 @@
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B819">
         <v>46</v>
@@ -12685,7 +12685,7 @@
     </row>
     <row r="820" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B820">
         <v>46</v>
@@ -12699,7 +12699,7 @@
     </row>
     <row r="821" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B821">
         <v>46</v>
@@ -12713,7 +12713,7 @@
     </row>
     <row r="822" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B822">
         <v>46</v>
@@ -12727,7 +12727,7 @@
     </row>
     <row r="823" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B823">
         <v>46</v>
@@ -12741,7 +12741,7 @@
     </row>
     <row r="824" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B824">
         <v>46</v>
@@ -12755,7 +12755,7 @@
     </row>
     <row r="825" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B825">
         <v>46</v>
@@ -12769,7 +12769,7 @@
     </row>
     <row r="826" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B826">
         <v>46</v>
@@ -12783,7 +12783,7 @@
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B827">
         <v>50</v>
@@ -12797,7 +12797,7 @@
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B828">
         <v>50</v>
@@ -12811,7 +12811,7 @@
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B829">
         <v>50</v>
@@ -12825,7 +12825,7 @@
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B830">
         <v>50</v>
@@ -12839,7 +12839,7 @@
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B831">
         <v>50</v>
@@ -12853,7 +12853,7 @@
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B832">
         <v>50</v>
@@ -12867,7 +12867,7 @@
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B833">
         <v>51</v>
@@ -12881,7 +12881,7 @@
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B834">
         <v>51</v>
@@ -12895,7 +12895,7 @@
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B835">
         <v>51</v>
@@ -12909,7 +12909,7 @@
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B836">
         <v>51</v>
@@ -12923,7 +12923,7 @@
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B837">
         <v>51</v>
@@ -12937,7 +12937,7 @@
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B838">
         <v>51</v>
@@ -12951,7 +12951,7 @@
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B839">
         <v>51</v>
@@ -12965,7 +12965,7 @@
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B840">
         <v>51</v>
@@ -12979,7 +12979,7 @@
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B841">
         <v>51</v>
@@ -12993,7 +12993,7 @@
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B842">
         <v>51</v>
@@ -13007,7 +13007,7 @@
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B843">
         <v>51</v>
@@ -13021,7 +13021,7 @@
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B844">
         <v>52</v>
@@ -13035,7 +13035,7 @@
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B845">
         <v>52</v>
@@ -13049,7 +13049,7 @@
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B846">
         <v>52</v>
@@ -13063,7 +13063,7 @@
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B847">
         <v>52</v>
@@ -13077,7 +13077,7 @@
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B848">
         <v>53</v>
@@ -13091,7 +13091,7 @@
     </row>
     <row r="849" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B849">
         <v>53</v>
@@ -13105,7 +13105,7 @@
     </row>
     <row r="850" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B850">
         <v>53</v>
@@ -13119,7 +13119,7 @@
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B851">
         <v>53</v>
@@ -13133,7 +13133,7 @@
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B852">
         <v>54</v>
@@ -13147,7 +13147,7 @@
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B853">
         <v>54</v>
@@ -13161,7 +13161,7 @@
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B854">
         <v>54</v>
@@ -13175,7 +13175,7 @@
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B855">
         <v>54</v>
@@ -13189,7 +13189,7 @@
     </row>
     <row r="856" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B856">
         <v>55</v>
@@ -13203,7 +13203,7 @@
     </row>
     <row r="857" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B857">
         <v>55</v>
@@ -13217,7 +13217,7 @@
     </row>
     <row r="858" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B858">
         <v>55</v>
@@ -13231,7 +13231,7 @@
     </row>
     <row r="859" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B859">
         <v>64</v>
@@ -13245,7 +13245,7 @@
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B860">
         <v>8</v>
@@ -13259,7 +13259,7 @@
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B861">
         <v>22</v>
@@ -13273,7 +13273,7 @@
     </row>
     <row r="862" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B862">
         <v>24</v>
@@ -13287,7 +13287,7 @@
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B863">
         <v>28</v>
@@ -13301,7 +13301,7 @@
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B864">
         <v>31</v>
@@ -13315,7 +13315,7 @@
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B865">
         <v>36</v>
@@ -13329,7 +13329,7 @@
     </row>
     <row r="866" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B866">
         <v>37</v>
@@ -13343,7 +13343,7 @@
     </row>
     <row r="867" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B867">
         <v>43</v>
@@ -13357,7 +13357,7 @@
     </row>
     <row r="868" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B868">
         <v>44</v>
@@ -13371,7 +13371,7 @@
     </row>
     <row r="869" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B869">
         <v>46</v>
@@ -13385,7 +13385,7 @@
     </row>
     <row r="870" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B870">
         <v>50</v>
@@ -13399,7 +13399,7 @@
     </row>
     <row r="871" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B871">
         <v>64</v>

</xml_diff>